<commit_message>
10 nodes 300 sec 90 prob - results
</commit_message>
<xml_diff>
--- a/results_epidemic_90.xlsx
+++ b/results_epidemic_90.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\study\web-simulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C08061FB-E054-427A-8FF7-DBFB91F50C22}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2C5E57A-ACAA-4D52-A9CA-8D15B8E8F417}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4E5B6BB3-DEEF-4635-8454-C81C003D43E3}"/>
+    <workbookView xWindow="1872" yWindow="1428" windowWidth="6252" windowHeight="8976" xr2:uid="{4E5B6BB3-DEEF-4635-8454-C81C003D43E3}"/>
   </bookViews>
   <sheets>
     <sheet name="10nodes" sheetId="1" r:id="rId1"/>
@@ -418,7 +418,7 @@
   <dimension ref="A1:I104"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:H102"/>
+      <selection activeCell="A103" sqref="A103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -454,6 +454,512 @@
         <v>2</v>
       </c>
     </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>4</v>
+      </c>
+      <c r="B44">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A70">
+        <v>2</v>
+      </c>
+      <c r="B70">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A102">
+        <v>0</v>
+      </c>
+    </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>3</v>
@@ -484,17 +990,17 @@
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A104" t="e">
+      <c r="A104">
         <f>AVERAGEIF(A3:A102, "&lt;&gt;0")</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="B104" t="e">
+        <v>3</v>
+      </c>
+      <c r="B104">
         <f>AVERAGEIF(B3:B102, "&lt;&gt;0")</f>
-        <v>#DIV/0!</v>
+        <v>293</v>
       </c>
       <c r="C104">
         <f>COUNTIF(A3:A102, "&lt;&gt;0")/100</f>
-        <v>1</v>
+        <v>0.02</v>
       </c>
       <c r="D104" t="e">
         <f>AVERAGEIF(D3:D102, "&lt;&gt;0")</f>

</xml_diff>

<commit_message>
20 nodes all time 90 prob - results
</commit_message>
<xml_diff>
--- a/results_epidemic_90.xlsx
+++ b/results_epidemic_90.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\study\web-simulator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daure\Desktop\DF\STUDY\web-simulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2C5E57A-ACAA-4D52-A9CA-8D15B8E8F417}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A556667A-3231-4C68-9073-DB05E86513A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1872" yWindow="1428" windowWidth="6252" windowHeight="8976" xr2:uid="{4E5B6BB3-DEEF-4635-8454-C81C003D43E3}"/>
+    <workbookView xWindow="888" yWindow="1320" windowWidth="8280" windowHeight="8868" activeTab="1" xr2:uid="{4E5B6BB3-DEEF-4635-8454-C81C003D43E3}"/>
   </bookViews>
   <sheets>
     <sheet name="10nodes" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,11 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -103,7 +107,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -119,9 +123,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -159,7 +163,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -265,7 +269,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -417,8 +421,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0BF19DE-A9AD-4CEB-8AC5-539E8A0C5820}">
   <dimension ref="A1:I104"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A103" sqref="A103"/>
+    <sheetView topLeftCell="C85" workbookViewId="0">
+      <selection activeCell="G103" sqref="G103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -458,505 +462,1195 @@
       <c r="A3">
         <v>0</v>
       </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>0</v>
       </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>0</v>
       </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>0</v>
       </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>0</v>
       </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>4</v>
+      </c>
+      <c r="H7">
+        <v>805</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>0</v>
       </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>0</v>
       </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>0</v>
       </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>0</v>
       </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>3</v>
+      </c>
+      <c r="H11">
+        <v>788</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>0</v>
       </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>4</v>
+      </c>
+      <c r="H12">
+        <v>585</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>0</v>
       </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>0</v>
       </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>0</v>
       </c>
+      <c r="D15">
+        <v>4</v>
+      </c>
+      <c r="E15">
+        <v>457</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16">
+        <v>502</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>3</v>
+      </c>
+      <c r="H20">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <v>4</v>
+      </c>
+      <c r="H29">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>4</v>
+      </c>
+      <c r="H31">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D32">
+        <v>3</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <v>4</v>
+      </c>
+      <c r="H34">
+        <v>824</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="G36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="G37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D38">
+        <v>0</v>
+      </c>
+      <c r="G38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="G39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="G41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D42">
+        <v>2</v>
+      </c>
+      <c r="E42">
+        <v>399</v>
+      </c>
+      <c r="G42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="G43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>4</v>
       </c>
       <c r="B44">
         <v>297</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D44">
+        <v>0</v>
+      </c>
+      <c r="G44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="G45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D46">
+        <v>0</v>
+      </c>
+      <c r="G46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D47">
+        <v>0</v>
+      </c>
+      <c r="G47">
+        <v>6</v>
+      </c>
+      <c r="H47">
+        <v>852</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D48">
+        <v>0</v>
+      </c>
+      <c r="G48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D49">
+        <v>0</v>
+      </c>
+      <c r="G49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D50">
+        <v>0</v>
+      </c>
+      <c r="G50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D51">
+        <v>0</v>
+      </c>
+      <c r="G51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D52">
+        <v>0</v>
+      </c>
+      <c r="G52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D53">
+        <v>2</v>
+      </c>
+      <c r="E53">
+        <v>399</v>
+      </c>
+      <c r="G53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D54">
+        <v>0</v>
+      </c>
+      <c r="G54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D55">
+        <v>0</v>
+      </c>
+      <c r="G55">
+        <v>4</v>
+      </c>
+      <c r="H55">
+        <v>888</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D56">
+        <v>0</v>
+      </c>
+      <c r="G56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D57">
+        <v>0</v>
+      </c>
+      <c r="G57">
+        <v>5</v>
+      </c>
+      <c r="H57">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D58">
+        <v>0</v>
+      </c>
+      <c r="G58">
+        <v>3</v>
+      </c>
+      <c r="H58">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D59">
+        <v>0</v>
+      </c>
+      <c r="G59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D60">
+        <v>0</v>
+      </c>
+      <c r="G60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D61">
+        <v>0</v>
+      </c>
+      <c r="G61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D62">
+        <v>0</v>
+      </c>
+      <c r="G62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D63">
+        <v>0</v>
+      </c>
+      <c r="G63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D64">
+        <v>0</v>
+      </c>
+      <c r="G64">
+        <v>4</v>
+      </c>
+      <c r="H64">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D65">
+        <v>0</v>
+      </c>
+      <c r="G65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D66">
+        <v>0</v>
+      </c>
+      <c r="G66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>0</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D67">
+        <v>0</v>
+      </c>
+      <c r="G67">
+        <v>3</v>
+      </c>
+      <c r="H67">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>0</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D68">
+        <v>0</v>
+      </c>
+      <c r="G68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>0</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D69">
+        <v>0</v>
+      </c>
+      <c r="G69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>2</v>
       </c>
       <c r="B70">
         <v>289</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D70">
+        <v>0</v>
+      </c>
+      <c r="G70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>0</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D71">
+        <v>0</v>
+      </c>
+      <c r="G71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>0</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D72">
+        <v>0</v>
+      </c>
+      <c r="G72">
+        <v>3</v>
+      </c>
+      <c r="H72">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>0</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D73">
+        <v>0</v>
+      </c>
+      <c r="G73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>0</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D74">
+        <v>0</v>
+      </c>
+      <c r="G74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>0</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D75">
+        <v>0</v>
+      </c>
+      <c r="G75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>0</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D76">
+        <v>0</v>
+      </c>
+      <c r="G76">
+        <v>4</v>
+      </c>
+      <c r="H76">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>0</v>
       </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D77">
+        <v>0</v>
+      </c>
+      <c r="G77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>0</v>
       </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D78">
+        <v>0</v>
+      </c>
+      <c r="G78">
+        <v>4</v>
+      </c>
+      <c r="H78">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>0</v>
       </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D79">
+        <v>0</v>
+      </c>
+      <c r="G79">
+        <v>5</v>
+      </c>
+      <c r="H79">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>0</v>
       </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D80">
+        <v>0</v>
+      </c>
+      <c r="G80">
+        <v>3</v>
+      </c>
+      <c r="H80">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>0</v>
       </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D81">
+        <v>2</v>
+      </c>
+      <c r="E81">
+        <v>311</v>
+      </c>
+      <c r="G81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>0</v>
       </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D82">
+        <v>0</v>
+      </c>
+      <c r="G82">
+        <v>4</v>
+      </c>
+      <c r="H82">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>0</v>
       </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D83">
+        <v>0</v>
+      </c>
+      <c r="G83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>0</v>
       </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D84">
+        <v>0</v>
+      </c>
+      <c r="G84">
+        <v>2</v>
+      </c>
+      <c r="H84">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>0</v>
       </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D85">
+        <v>0</v>
+      </c>
+      <c r="G85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>0</v>
       </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D86">
+        <v>0</v>
+      </c>
+      <c r="G86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>0</v>
       </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D87">
+        <v>0</v>
+      </c>
+      <c r="G87">
+        <v>3</v>
+      </c>
+      <c r="H87">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>0</v>
       </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D88">
+        <v>0</v>
+      </c>
+      <c r="G88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>0</v>
       </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D89">
+        <v>0</v>
+      </c>
+      <c r="G89">
+        <v>4</v>
+      </c>
+      <c r="H89">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>0</v>
       </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D90">
+        <v>0</v>
+      </c>
+      <c r="G90">
+        <v>4</v>
+      </c>
+      <c r="H90">
+        <v>897</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>0</v>
       </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D91">
+        <v>0</v>
+      </c>
+      <c r="G91">
+        <v>2</v>
+      </c>
+      <c r="H91">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>0</v>
       </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D92">
+        <v>0</v>
+      </c>
+      <c r="G92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>0</v>
       </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D93">
+        <v>0</v>
+      </c>
+      <c r="G93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>0</v>
       </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D94">
+        <v>0</v>
+      </c>
+      <c r="G94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>0</v>
       </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D95">
+        <v>0</v>
+      </c>
+      <c r="G95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>0</v>
+      </c>
+      <c r="D96">
+        <v>0</v>
+      </c>
+      <c r="G96">
+        <v>4</v>
+      </c>
+      <c r="H96">
+        <v>713</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>0</v>
       </c>
+      <c r="D97">
+        <v>0</v>
+      </c>
+      <c r="G97">
+        <v>0</v>
+      </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>0</v>
       </c>
+      <c r="D98">
+        <v>0</v>
+      </c>
+      <c r="G98">
+        <v>0</v>
+      </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>0</v>
       </c>
+      <c r="D99">
+        <v>0</v>
+      </c>
+      <c r="G99">
+        <v>0</v>
+      </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>0</v>
       </c>
+      <c r="D100">
+        <v>0</v>
+      </c>
+      <c r="G100">
+        <v>0</v>
+      </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>0</v>
       </c>
+      <c r="D101">
+        <v>0</v>
+      </c>
+      <c r="G101">
+        <v>0</v>
+      </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A102">
+        <v>0</v>
+      </c>
+      <c r="D102">
+        <v>0</v>
+      </c>
+      <c r="G102">
         <v>0</v>
       </c>
     </row>
@@ -1002,29 +1696,29 @@
         <f>COUNTIF(A3:A102, "&lt;&gt;0")/100</f>
         <v>0.02</v>
       </c>
-      <c r="D104" t="e">
+      <c r="D104">
         <f>AVERAGEIF(D3:D102, "&lt;&gt;0")</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E104" t="e">
+        <v>2.5</v>
+      </c>
+      <c r="E104">
         <f>AVERAGE(E3:E102)</f>
-        <v>#DIV/0!</v>
+        <v>413.6</v>
       </c>
       <c r="F104">
         <f>COUNTIF(D3:D102, "&lt;&gt;0")/100</f>
-        <v>1</v>
-      </c>
-      <c r="G104" t="e">
+        <v>0.06</v>
+      </c>
+      <c r="G104">
         <f>AVERAGEIF(G3:G102, "&lt;&gt;0")</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H104" t="e">
+        <v>3.72</v>
+      </c>
+      <c r="H104">
         <f>AVERAGE(H3:H102)</f>
-        <v>#DIV/0!</v>
+        <v>656.92</v>
       </c>
       <c r="I104">
         <f>COUNTIF(G3:G102, "&lt;&gt;0")/100</f>
-        <v>1</v>
+        <v>0.25</v>
       </c>
     </row>
   </sheetData>
@@ -1036,8 +1730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB1E408E-911F-40D8-9CD7-6D7E9E262C6C}">
   <dimension ref="A1:I104"/>
   <sheetViews>
-    <sheetView topLeftCell="A96" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:H102"/>
+    <sheetView tabSelected="1" topLeftCell="C94" workbookViewId="0">
+      <selection activeCell="G103" sqref="G103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1073,6 +1767,1280 @@
         <v>2</v>
       </c>
     </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>4</v>
+      </c>
+      <c r="H4">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>5</v>
+      </c>
+      <c r="H6">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>3</v>
+      </c>
+      <c r="H10">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>6</v>
+      </c>
+      <c r="E16">
+        <v>556</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>2</v>
+      </c>
+      <c r="E19">
+        <v>346</v>
+      </c>
+      <c r="G19">
+        <v>3</v>
+      </c>
+      <c r="H19">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>2</v>
+      </c>
+      <c r="E21">
+        <v>297</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>4</v>
+      </c>
+      <c r="H25">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>5</v>
+      </c>
+      <c r="H26">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>3</v>
+      </c>
+      <c r="H27">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>3</v>
+      </c>
+      <c r="E29">
+        <v>528</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <v>2</v>
+      </c>
+      <c r="H30">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>5</v>
+      </c>
+      <c r="E34">
+        <v>534</v>
+      </c>
+      <c r="G34">
+        <v>4</v>
+      </c>
+      <c r="H34">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="G36">
+        <v>4</v>
+      </c>
+      <c r="H36">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="G37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+      <c r="G38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="G39">
+        <v>2</v>
+      </c>
+      <c r="H39">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>0</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>0</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="G41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>0</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="G42">
+        <v>2</v>
+      </c>
+      <c r="H42">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>0</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="G43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>0</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+      <c r="G44">
+        <v>2</v>
+      </c>
+      <c r="H44">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>0</v>
+      </c>
+      <c r="D45">
+        <v>4</v>
+      </c>
+      <c r="E45">
+        <v>534</v>
+      </c>
+      <c r="G45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>0</v>
+      </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
+      <c r="G46">
+        <v>3</v>
+      </c>
+      <c r="H46">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>0</v>
+      </c>
+      <c r="D47">
+        <v>5</v>
+      </c>
+      <c r="E47">
+        <v>590</v>
+      </c>
+      <c r="G47">
+        <v>2</v>
+      </c>
+      <c r="H47">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>0</v>
+      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+      <c r="G48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>0</v>
+      </c>
+      <c r="D49">
+        <v>0</v>
+      </c>
+      <c r="G49">
+        <v>4</v>
+      </c>
+      <c r="H49">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>0</v>
+      </c>
+      <c r="D50">
+        <v>3</v>
+      </c>
+      <c r="E50">
+        <v>587</v>
+      </c>
+      <c r="G50">
+        <v>2</v>
+      </c>
+      <c r="H50">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>0</v>
+      </c>
+      <c r="D51">
+        <v>0</v>
+      </c>
+      <c r="G51">
+        <v>2</v>
+      </c>
+      <c r="H51">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>0</v>
+      </c>
+      <c r="D52">
+        <v>0</v>
+      </c>
+      <c r="G52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>0</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+      <c r="G53">
+        <v>3</v>
+      </c>
+      <c r="H53">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>0</v>
+      </c>
+      <c r="D54">
+        <v>0</v>
+      </c>
+      <c r="G54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>0</v>
+      </c>
+      <c r="D55">
+        <v>0</v>
+      </c>
+      <c r="G55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
+      <c r="G56">
+        <v>3</v>
+      </c>
+      <c r="H56">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>0</v>
+      </c>
+      <c r="D57">
+        <v>0</v>
+      </c>
+      <c r="G57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>0</v>
+      </c>
+      <c r="D58">
+        <v>0</v>
+      </c>
+      <c r="G58">
+        <v>2</v>
+      </c>
+      <c r="H58">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>0</v>
+      </c>
+      <c r="D59">
+        <v>0</v>
+      </c>
+      <c r="G59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>0</v>
+      </c>
+      <c r="D60">
+        <v>0</v>
+      </c>
+      <c r="G60">
+        <v>2</v>
+      </c>
+      <c r="H60">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>0</v>
+      </c>
+      <c r="D61">
+        <v>0</v>
+      </c>
+      <c r="G61">
+        <v>2</v>
+      </c>
+      <c r="H61">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>0</v>
+      </c>
+      <c r="D62">
+        <v>0</v>
+      </c>
+      <c r="G62">
+        <v>2</v>
+      </c>
+      <c r="H62">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>0</v>
+      </c>
+      <c r="D63">
+        <v>0</v>
+      </c>
+      <c r="G63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>0</v>
+      </c>
+      <c r="D64">
+        <v>2</v>
+      </c>
+      <c r="E64">
+        <v>352</v>
+      </c>
+      <c r="G64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>0</v>
+      </c>
+      <c r="D65">
+        <v>0</v>
+      </c>
+      <c r="G65">
+        <v>4</v>
+      </c>
+      <c r="H65">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>0</v>
+      </c>
+      <c r="D66">
+        <v>0</v>
+      </c>
+      <c r="G66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <v>0</v>
+      </c>
+      <c r="D67">
+        <v>0</v>
+      </c>
+      <c r="G67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <v>0</v>
+      </c>
+      <c r="D68">
+        <v>0</v>
+      </c>
+      <c r="G68">
+        <v>3</v>
+      </c>
+      <c r="H68">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A69">
+        <v>0</v>
+      </c>
+      <c r="D69">
+        <v>0</v>
+      </c>
+      <c r="G69">
+        <v>4</v>
+      </c>
+      <c r="H69">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A70">
+        <v>0</v>
+      </c>
+      <c r="D70">
+        <v>3</v>
+      </c>
+      <c r="E70">
+        <v>576</v>
+      </c>
+      <c r="G70">
+        <v>2</v>
+      </c>
+      <c r="H70">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A71">
+        <v>0</v>
+      </c>
+      <c r="D71">
+        <v>0</v>
+      </c>
+      <c r="G71">
+        <v>7</v>
+      </c>
+      <c r="H71">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A72">
+        <v>0</v>
+      </c>
+      <c r="D72">
+        <v>0</v>
+      </c>
+      <c r="G72">
+        <v>6</v>
+      </c>
+      <c r="H72">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A73">
+        <v>0</v>
+      </c>
+      <c r="D73">
+        <v>0</v>
+      </c>
+      <c r="G73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A74">
+        <v>2</v>
+      </c>
+      <c r="B74">
+        <v>298</v>
+      </c>
+      <c r="D74">
+        <v>0</v>
+      </c>
+      <c r="G74">
+        <v>5</v>
+      </c>
+      <c r="H74">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A75">
+        <v>0</v>
+      </c>
+      <c r="D75">
+        <v>0</v>
+      </c>
+      <c r="G75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A76">
+        <v>0</v>
+      </c>
+      <c r="D76">
+        <v>0</v>
+      </c>
+      <c r="G76">
+        <v>4</v>
+      </c>
+      <c r="H76">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A77">
+        <v>0</v>
+      </c>
+      <c r="D77">
+        <v>0</v>
+      </c>
+      <c r="G77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A78">
+        <v>0</v>
+      </c>
+      <c r="D78">
+        <v>2</v>
+      </c>
+      <c r="E78">
+        <v>299</v>
+      </c>
+      <c r="G78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A79">
+        <v>0</v>
+      </c>
+      <c r="D79">
+        <v>0</v>
+      </c>
+      <c r="G79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A80">
+        <v>0</v>
+      </c>
+      <c r="D80">
+        <v>3</v>
+      </c>
+      <c r="E80">
+        <v>389</v>
+      </c>
+      <c r="G80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A81">
+        <v>0</v>
+      </c>
+      <c r="D81">
+        <v>0</v>
+      </c>
+      <c r="G81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A82">
+        <v>0</v>
+      </c>
+      <c r="D82">
+        <v>0</v>
+      </c>
+      <c r="G82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A83">
+        <v>0</v>
+      </c>
+      <c r="D83">
+        <v>0</v>
+      </c>
+      <c r="G83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A84">
+        <v>0</v>
+      </c>
+      <c r="D84">
+        <v>0</v>
+      </c>
+      <c r="G84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A85">
+        <v>0</v>
+      </c>
+      <c r="D85">
+        <v>0</v>
+      </c>
+      <c r="G85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A86">
+        <v>0</v>
+      </c>
+      <c r="D86">
+        <v>0</v>
+      </c>
+      <c r="G86">
+        <v>7</v>
+      </c>
+      <c r="H86">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A87">
+        <v>3</v>
+      </c>
+      <c r="B87">
+        <v>299</v>
+      </c>
+      <c r="D87">
+        <v>0</v>
+      </c>
+      <c r="G87">
+        <v>3</v>
+      </c>
+      <c r="H87">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A88">
+        <v>0</v>
+      </c>
+      <c r="D88">
+        <v>0</v>
+      </c>
+      <c r="G88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A89">
+        <v>0</v>
+      </c>
+      <c r="D89">
+        <v>4</v>
+      </c>
+      <c r="E89">
+        <v>578</v>
+      </c>
+      <c r="G89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A90">
+        <v>0</v>
+      </c>
+      <c r="D90">
+        <v>0</v>
+      </c>
+      <c r="G90">
+        <v>3</v>
+      </c>
+      <c r="H90">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A91">
+        <v>0</v>
+      </c>
+      <c r="D91">
+        <v>0</v>
+      </c>
+      <c r="G91">
+        <v>4</v>
+      </c>
+      <c r="H91">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A92">
+        <v>0</v>
+      </c>
+      <c r="D92">
+        <v>0</v>
+      </c>
+      <c r="G92">
+        <v>5</v>
+      </c>
+      <c r="H92">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A93">
+        <v>0</v>
+      </c>
+      <c r="D93">
+        <v>0</v>
+      </c>
+      <c r="G93">
+        <v>3</v>
+      </c>
+      <c r="H93">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A94">
+        <v>0</v>
+      </c>
+      <c r="D94">
+        <v>0</v>
+      </c>
+      <c r="G94">
+        <v>2</v>
+      </c>
+      <c r="H94">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A95">
+        <v>0</v>
+      </c>
+      <c r="D95">
+        <v>0</v>
+      </c>
+      <c r="G95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A96">
+        <v>0</v>
+      </c>
+      <c r="D96">
+        <v>0</v>
+      </c>
+      <c r="G96">
+        <v>5</v>
+      </c>
+      <c r="H96">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A97">
+        <v>0</v>
+      </c>
+      <c r="D97">
+        <v>0</v>
+      </c>
+      <c r="G97">
+        <v>3</v>
+      </c>
+      <c r="H97">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A98">
+        <v>0</v>
+      </c>
+      <c r="D98">
+        <v>0</v>
+      </c>
+      <c r="G98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A99">
+        <v>0</v>
+      </c>
+      <c r="D99">
+        <v>3</v>
+      </c>
+      <c r="E99">
+        <v>430</v>
+      </c>
+      <c r="G99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A100">
+        <v>0</v>
+      </c>
+      <c r="D100">
+        <v>0</v>
+      </c>
+      <c r="G100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A101">
+        <v>0</v>
+      </c>
+      <c r="D101">
+        <v>0</v>
+      </c>
+      <c r="G101">
+        <v>2</v>
+      </c>
+      <c r="H101">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A102">
+        <v>0</v>
+      </c>
+      <c r="D102">
+        <v>0</v>
+      </c>
+      <c r="G102">
+        <v>0</v>
+      </c>
+    </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>3</v>
@@ -1103,41 +3071,41 @@
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A104" t="e">
+      <c r="A104">
         <f>AVERAGEIF(A3:A102, "&lt;&gt;0")</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="B104" t="e">
+        <v>2.5</v>
+      </c>
+      <c r="B104">
         <f>AVERAGEIF(B3:B102, "&lt;&gt;0")</f>
-        <v>#DIV/0!</v>
+        <v>298.5</v>
       </c>
       <c r="C104">
         <f>COUNTIF(A3:A102, "&lt;&gt;0")/100</f>
-        <v>1</v>
-      </c>
-      <c r="D104" t="e">
+        <v>0.02</v>
+      </c>
+      <c r="D104">
         <f>AVERAGEIF(D3:D102, "&lt;&gt;0")</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E104" t="e">
+        <v>3.3571428571428572</v>
+      </c>
+      <c r="E104">
         <f>AVERAGEIF(E3:E102, "&lt;&gt;0")</f>
-        <v>#DIV/0!</v>
+        <v>471.14285714285717</v>
       </c>
       <c r="F104">
         <f>COUNTIF(D3:D102, "&lt;&gt;0")/100</f>
-        <v>1</v>
-      </c>
-      <c r="G104" t="e">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="G104">
         <f>AVERAGEIF(G3:G102, "&lt;&gt;0")</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H104" t="e">
+        <v>3.3809523809523809</v>
+      </c>
+      <c r="H104">
         <f>AVERAGEIF(H3:H102, "&lt;&gt;0")</f>
-        <v>#DIV/0!</v>
+        <v>612.33333333333337</v>
       </c>
       <c r="I104">
         <f>COUNTIF(G3:G102, "&lt;&gt;0")/100</f>
-        <v>1</v>
+        <v>0.42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
30 nodes 90 prob 300 sec - results
</commit_message>
<xml_diff>
--- a/results_epidemic_90.xlsx
+++ b/results_epidemic_90.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daure\Desktop\DF\STUDY\web-simulator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\study\web-simulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A556667A-3231-4C68-9073-DB05E86513A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A6681B9-99CE-4557-B73C-D9F587F58A1B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="888" yWindow="1320" windowWidth="8280" windowHeight="8868" activeTab="1" xr2:uid="{4E5B6BB3-DEEF-4635-8454-C81C003D43E3}"/>
+    <workbookView xWindow="948" yWindow="1320" windowWidth="6252" windowHeight="8976" activeTab="2" xr2:uid="{4E5B6BB3-DEEF-4635-8454-C81C003D43E3}"/>
   </bookViews>
   <sheets>
     <sheet name="10nodes" sheetId="1" r:id="rId1"/>
@@ -25,11 +25,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -107,7 +103,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -123,9 +119,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -163,7 +159,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -269,7 +265,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1730,7 +1726,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB1E408E-911F-40D8-9CD7-6D7E9E262C6C}">
   <dimension ref="A1:I104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C94" workbookViewId="0">
+    <sheetView topLeftCell="C81" workbookViewId="0">
       <selection activeCell="G103" sqref="G103"/>
     </sheetView>
   </sheetViews>
@@ -3117,8 +3113,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E80694E4-B31D-4F12-997C-9508F4349611}">
   <dimension ref="A1:I104"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3154,6 +3150,512 @@
         <v>2</v>
       </c>
     </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>3</v>
+      </c>
+      <c r="B59">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A102">
+        <v>2</v>
+      </c>
+      <c r="B102">
+        <v>291</v>
+      </c>
+    </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>3</v>
@@ -3184,17 +3686,17 @@
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A104" t="e">
+      <c r="A104">
         <f>AVERAGEIF(A3:A102, "&lt;&gt;0")</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="B104" t="e">
+        <v>2.5</v>
+      </c>
+      <c r="B104">
         <f>AVERAGE(B3:B102)</f>
-        <v>#DIV/0!</v>
+        <v>294.5</v>
       </c>
       <c r="C104">
         <f>COUNTIF(A3:A102, "&lt;&gt;0")/100</f>
-        <v>1</v>
+        <v>0.02</v>
       </c>
       <c r="D104" t="e">
         <f>AVERAGEIF(D3:D102, "&lt;&gt;0")</f>

</xml_diff>

<commit_message>
90 prob for epidemic - results
</commit_message>
<xml_diff>
--- a/results_epidemic_90.xlsx
+++ b/results_epidemic_90.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\study\web-simulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A6681B9-99CE-4557-B73C-D9F587F58A1B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C106692-E78E-493A-8C86-E00C39AB30E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="948" yWindow="1320" windowWidth="6252" windowHeight="8976" activeTab="2" xr2:uid="{4E5B6BB3-DEEF-4635-8454-C81C003D43E3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{4E5B6BB3-DEEF-4635-8454-C81C003D43E3}"/>
   </bookViews>
   <sheets>
     <sheet name="10nodes" sheetId="1" r:id="rId1"/>
@@ -417,8 +417,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0BF19DE-A9AD-4CEB-8AC5-539E8A0C5820}">
   <dimension ref="A1:I104"/>
   <sheetViews>
-    <sheetView topLeftCell="C85" workbookViewId="0">
-      <selection activeCell="G103" sqref="G103"/>
+    <sheetView topLeftCell="A81" workbookViewId="0">
+      <selection activeCell="H91" sqref="G89:H91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1726,8 +1726,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB1E408E-911F-40D8-9CD7-6D7E9E262C6C}">
   <dimension ref="A1:I104"/>
   <sheetViews>
-    <sheetView topLeftCell="C81" workbookViewId="0">
-      <selection activeCell="G103" sqref="G103"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="G91" sqref="G91:H93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3113,8 +3113,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E80694E4-B31D-4F12-997C-9508F4349611}">
   <dimension ref="A1:I104"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView topLeftCell="A86" workbookViewId="0">
+      <selection activeCell="I104" sqref="I104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3154,472 +3154,1228 @@
       <c r="A3">
         <v>0</v>
       </c>
+      <c r="D3">
+        <v>4</v>
+      </c>
+      <c r="E3">
+        <v>544</v>
+      </c>
+      <c r="G3">
+        <v>6</v>
+      </c>
+      <c r="H3">
+        <v>714</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>0</v>
       </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>4</v>
+      </c>
+      <c r="H4">
+        <v>779</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>0</v>
       </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <v>593</v>
+      </c>
+      <c r="G5">
+        <v>3</v>
+      </c>
+      <c r="H5">
+        <v>429</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>0</v>
       </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>0</v>
       </c>
+      <c r="D7">
+        <v>5</v>
+      </c>
+      <c r="E7">
+        <v>507</v>
+      </c>
+      <c r="G7">
+        <v>3</v>
+      </c>
+      <c r="H7">
+        <v>635</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>0</v>
       </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>0</v>
       </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>6</v>
+      </c>
+      <c r="H9">
+        <v>837</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>0</v>
       </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>0</v>
       </c>
+      <c r="D11">
+        <v>5</v>
+      </c>
+      <c r="E11">
+        <v>367</v>
+      </c>
+      <c r="G11">
+        <v>4</v>
+      </c>
+      <c r="H11">
+        <v>844</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>0</v>
       </c>
+      <c r="D12">
+        <v>3</v>
+      </c>
+      <c r="E12">
+        <v>567</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>0</v>
       </c>
+      <c r="D13">
+        <v>4</v>
+      </c>
+      <c r="E13">
+        <v>541</v>
+      </c>
+      <c r="G13">
+        <v>2</v>
+      </c>
+      <c r="H13">
+        <v>808</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>0</v>
       </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>6</v>
+      </c>
+      <c r="H14">
+        <v>491</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>0</v>
       </c>
+      <c r="D15">
+        <v>5</v>
+      </c>
+      <c r="E15">
+        <v>600</v>
+      </c>
+      <c r="G15">
+        <v>5</v>
+      </c>
+      <c r="H15">
+        <v>377</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>5</v>
+      </c>
+      <c r="H17">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D19">
+        <v>6</v>
+      </c>
+      <c r="E19">
+        <v>536</v>
+      </c>
+      <c r="G19">
+        <v>2</v>
+      </c>
+      <c r="H19">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>5</v>
+      </c>
+      <c r="H24">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D25">
+        <v>3</v>
+      </c>
+      <c r="E25">
+        <v>567</v>
+      </c>
+      <c r="G25">
+        <v>3</v>
+      </c>
+      <c r="H25">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D26">
+        <v>3</v>
+      </c>
+      <c r="E26">
+        <v>457</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D27">
+        <v>3</v>
+      </c>
+      <c r="E27">
+        <v>472</v>
+      </c>
+      <c r="G27">
+        <v>3</v>
+      </c>
+      <c r="H27">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <v>5</v>
+      </c>
+      <c r="H29">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <v>4</v>
+      </c>
+      <c r="H30">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D32">
+        <v>4</v>
+      </c>
+      <c r="E32">
+        <v>551</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D33">
+        <v>2</v>
+      </c>
+      <c r="E33">
+        <v>327</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D34">
+        <v>5</v>
+      </c>
+      <c r="E34">
+        <v>542</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="G36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="G37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D38">
+        <v>0</v>
+      </c>
+      <c r="G38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D39">
+        <v>5</v>
+      </c>
+      <c r="E39">
+        <v>576</v>
+      </c>
+      <c r="G39">
+        <v>3</v>
+      </c>
+      <c r="H39">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D40">
+        <v>5</v>
+      </c>
+      <c r="E40">
+        <v>522</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="G41">
+        <v>5</v>
+      </c>
+      <c r="H41">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="G42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="G43">
+        <v>3</v>
+      </c>
+      <c r="H43">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D44">
+        <v>3</v>
+      </c>
+      <c r="E44">
+        <v>503</v>
+      </c>
+      <c r="G44">
+        <v>2</v>
+      </c>
+      <c r="H44">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="G45">
+        <v>4</v>
+      </c>
+      <c r="H45">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D46">
+        <v>0</v>
+      </c>
+      <c r="G46">
+        <v>4</v>
+      </c>
+      <c r="H46">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D47">
+        <v>0</v>
+      </c>
+      <c r="G47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D48">
+        <v>0</v>
+      </c>
+      <c r="G48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D49">
+        <v>0</v>
+      </c>
+      <c r="G49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D50">
+        <v>0</v>
+      </c>
+      <c r="G50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D51">
+        <v>0</v>
+      </c>
+      <c r="G51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D52">
+        <v>0</v>
+      </c>
+      <c r="G52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D53">
+        <v>0</v>
+      </c>
+      <c r="G53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D54">
+        <v>0</v>
+      </c>
+      <c r="G54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D55">
+        <v>0</v>
+      </c>
+      <c r="G55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D56">
+        <v>0</v>
+      </c>
+      <c r="G56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D57">
+        <v>4</v>
+      </c>
+      <c r="E57">
+        <v>419</v>
+      </c>
+      <c r="G57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D58">
+        <v>0</v>
+      </c>
+      <c r="G58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>3</v>
       </c>
       <c r="B59">
         <v>298</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D59">
+        <v>0</v>
+      </c>
+      <c r="G59">
+        <v>4</v>
+      </c>
+      <c r="H59">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D60">
+        <v>0</v>
+      </c>
+      <c r="G60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D61">
+        <v>0</v>
+      </c>
+      <c r="G61">
+        <v>7</v>
+      </c>
+      <c r="H61">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D62">
+        <v>0</v>
+      </c>
+      <c r="G62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D63">
+        <v>2</v>
+      </c>
+      <c r="E63">
+        <v>417</v>
+      </c>
+      <c r="G63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D64">
+        <v>0</v>
+      </c>
+      <c r="G64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D65">
+        <v>0</v>
+      </c>
+      <c r="G65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D66">
+        <v>0</v>
+      </c>
+      <c r="G66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>0</v>
       </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D67">
+        <v>0</v>
+      </c>
+      <c r="G67">
+        <v>3</v>
+      </c>
+      <c r="H67">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>0</v>
       </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D68">
+        <v>0</v>
+      </c>
+      <c r="G68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>0</v>
       </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D69">
+        <v>0</v>
+      </c>
+      <c r="G69">
+        <v>6</v>
+      </c>
+      <c r="H69">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>0</v>
       </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D70">
+        <v>0</v>
+      </c>
+      <c r="G70">
+        <v>3</v>
+      </c>
+      <c r="H70">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>0</v>
       </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D71">
+        <v>3</v>
+      </c>
+      <c r="E71">
+        <v>354</v>
+      </c>
+      <c r="G71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>0</v>
       </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D72">
+        <v>0</v>
+      </c>
+      <c r="G72">
+        <v>4</v>
+      </c>
+      <c r="H72">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>0</v>
       </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D73">
+        <v>0</v>
+      </c>
+      <c r="G73">
+        <v>3</v>
+      </c>
+      <c r="H73">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>0</v>
       </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D74">
+        <v>0</v>
+      </c>
+      <c r="G74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>0</v>
       </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D75">
+        <v>0</v>
+      </c>
+      <c r="G75">
+        <v>3</v>
+      </c>
+      <c r="H75">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>0</v>
       </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D76">
+        <v>0</v>
+      </c>
+      <c r="G76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>0</v>
       </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D77">
+        <v>0</v>
+      </c>
+      <c r="G77">
+        <v>3</v>
+      </c>
+      <c r="H77">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>0</v>
       </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D78">
+        <v>4</v>
+      </c>
+      <c r="E78">
+        <v>484</v>
+      </c>
+      <c r="G78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>0</v>
       </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D79">
+        <v>0</v>
+      </c>
+      <c r="G79">
+        <v>3</v>
+      </c>
+      <c r="H79">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>0</v>
       </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D80">
+        <v>5</v>
+      </c>
+      <c r="E80">
+        <v>477</v>
+      </c>
+      <c r="G80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>0</v>
       </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D81">
+        <v>4</v>
+      </c>
+      <c r="E81">
+        <v>461</v>
+      </c>
+      <c r="G81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>0</v>
       </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D82">
+        <v>4</v>
+      </c>
+      <c r="E82">
+        <v>477</v>
+      </c>
+      <c r="G82">
+        <v>4</v>
+      </c>
+      <c r="H82">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>0</v>
       </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D83">
+        <v>0</v>
+      </c>
+      <c r="G83">
+        <v>6</v>
+      </c>
+      <c r="H83">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>0</v>
       </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D84">
+        <v>0</v>
+      </c>
+      <c r="G84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>0</v>
       </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D85">
+        <v>0</v>
+      </c>
+      <c r="G85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>0</v>
       </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D86">
+        <v>0</v>
+      </c>
+      <c r="G86">
+        <v>3</v>
+      </c>
+      <c r="H86">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>0</v>
       </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D87">
+        <v>0</v>
+      </c>
+      <c r="G87">
+        <v>6</v>
+      </c>
+      <c r="H87">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>0</v>
       </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D88">
+        <v>3</v>
+      </c>
+      <c r="E88">
+        <v>428</v>
+      </c>
+      <c r="G88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>0</v>
       </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D89">
+        <v>0</v>
+      </c>
+      <c r="G89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>0</v>
       </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D90">
+        <v>0</v>
+      </c>
+      <c r="G90">
+        <v>6</v>
+      </c>
+      <c r="H90">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>0</v>
       </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D91">
+        <v>0</v>
+      </c>
+      <c r="G91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>0</v>
       </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D92">
+        <v>0</v>
+      </c>
+      <c r="G92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>0</v>
       </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D93">
+        <v>2</v>
+      </c>
+      <c r="E93">
+        <v>360</v>
+      </c>
+      <c r="G93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A94">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+      <c r="B94">
+        <v>296</v>
+      </c>
+      <c r="D94">
+        <v>0</v>
+      </c>
+      <c r="G94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>0</v>
       </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D95">
+        <v>0</v>
+      </c>
+      <c r="G95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A96">
+        <v>0</v>
+      </c>
+      <c r="D96">
+        <v>0</v>
+      </c>
+      <c r="G96">
         <v>0</v>
       </c>
     </row>
@@ -3627,24 +4383,63 @@
       <c r="A97">
         <v>0</v>
       </c>
+      <c r="D97">
+        <v>0</v>
+      </c>
+      <c r="G97">
+        <v>5</v>
+      </c>
+      <c r="H97">
+        <v>527</v>
+      </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>0</v>
       </c>
+      <c r="D98">
+        <v>0</v>
+      </c>
+      <c r="G98">
+        <v>7</v>
+      </c>
+      <c r="H98">
+        <v>576</v>
+      </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>0</v>
       </c>
+      <c r="D99">
+        <v>5</v>
+      </c>
+      <c r="E99">
+        <v>448</v>
+      </c>
+      <c r="G99">
+        <v>0</v>
+      </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>0</v>
       </c>
+      <c r="D100">
+        <v>0</v>
+      </c>
+      <c r="G100">
+        <v>0</v>
+      </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A101">
+        <v>0</v>
+      </c>
+      <c r="D101">
+        <v>0</v>
+      </c>
+      <c r="G101">
         <v>0</v>
       </c>
     </row>
@@ -3655,6 +4450,12 @@
       <c r="B102">
         <v>291</v>
       </c>
+      <c r="D102">
+        <v>0</v>
+      </c>
+      <c r="G102">
+        <v>0</v>
+      </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
@@ -3688,39 +4489,39 @@
     <row r="104" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A104">
         <f>AVERAGEIF(A3:A102, "&lt;&gt;0")</f>
-        <v>2.5</v>
+        <v>2.6666666666666665</v>
       </c>
       <c r="B104">
         <f>AVERAGE(B3:B102)</f>
-        <v>294.5</v>
+        <v>295</v>
       </c>
       <c r="C104">
         <f>COUNTIF(A3:A102, "&lt;&gt;0")/100</f>
-        <v>0.02</v>
-      </c>
-      <c r="D104" t="e">
+        <v>0.03</v>
+      </c>
+      <c r="D104">
         <f>AVERAGEIF(D3:D102, "&lt;&gt;0")</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E104" t="e">
+        <v>3.8888888888888888</v>
+      </c>
+      <c r="E104">
         <f>AVERAGEIF(E3:E102, "&lt;&gt;0")</f>
-        <v>#DIV/0!</v>
+        <v>485.07407407407408</v>
       </c>
       <c r="F104">
         <f>COUNTIF(D3:D102, "&lt;&gt;0")/100</f>
-        <v>1</v>
-      </c>
-      <c r="G104" t="e">
+        <v>0.27</v>
+      </c>
+      <c r="G104">
         <f>AVERAGEIF(G3:G102, "&lt;&gt;0")</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H104" t="e">
+        <v>4.1794871794871797</v>
+      </c>
+      <c r="H104">
         <f>AVERAGE(H3:H102)</f>
-        <v>#DIV/0!</v>
+        <v>623</v>
       </c>
       <c r="I104">
         <f>COUNTIF(G3:G102, "&lt;&gt;0")/100</f>
-        <v>1</v>
+        <v>0.39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>